<commit_message>
changes to crosswalks and data files
</commit_message>
<xml_diff>
--- a/Python/btax/depreciation/data/raw_data/soi/soi_proprietorship/farm_data.xlsx
+++ b/Python/btax/depreciation/data/raw_data/soi/soi_proprietorship/farm_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Lott, Sherwin\OLG Dynamic Scoring Model\Calibration\Draft 2\Program\data\SOI_Proprietorships\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\B-Tax\Python\btax\depreciation\data\raw_data\soi\soi_proprietorship\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -362,16 +362,16 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,24 +391,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>137987000</v>
+      </c>
+      <c r="B2">
         <v>1828946000</v>
       </c>
-      <c r="B2">
-        <v>137987000</v>
-      </c>
       <c r="C2">
+        <v>137929000</v>
+      </c>
+      <c r="D2">
         <v>1828272000</v>
       </c>
-      <c r="D2">
-        <v>137929000</v>
-      </c>
       <c r="E2">
+        <v>156076785</v>
+      </c>
+      <c r="F2">
         <v>562433686</v>
-      </c>
-      <c r="F2">
-        <v>156076785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>